<commit_message>
modified:   src/AAS.jl 	modified:   src/Anotation.jl 	modified:   src/ForestInventory.jl 	new file:   src/qml/images/correct.png 	new file:   src/qml/images/errado.png 	deleted:    src/qml/images/pasta.ico 	deleted:    src/qml/images/pasta.png 	modified:   src/qml/main.qml 	new file:   src/qml/tableview.qml 	modified:   teste.xlsx
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -93,7 +93,7 @@
     <t>População</t>
   </si>
   <si>
-    <t>A população avaliada é considerada finita</t>
+    <t>A população avaliada é considerada infinita</t>
   </si>
   <si>
     <t>Número total de unidades amostrais da população</t>
@@ -477,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.021797142857142862</v>
+        <v>21.79714285714286</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -485,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.018139946248662137</v>
+        <v>21.720718880312205</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.021920437724555514</v>
+        <v>21.720718880312205</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -501,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>9808.714285714288</v>
+        <v>217971.42857142858</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -509,7 +509,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>8958.103703638279</v>
+        <v>217971.42857142858</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -517,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>10.659324867790296</v>
+        <v>217971.42857142858</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -525,7 +525,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>4.346980377481729</v>
+        <v>4.71386089662237</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -533,7 +533,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>45.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -541,7 +541,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.0018902457379466869</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -549,7 +549,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.0009475175228516604</v>
+        <v>1.0274869937237732</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -557,7 +557,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.008626819848816466</v>
+        <v>8.626819848816465</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -565,7 +565,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>7.442202070393374e-5</v>
+        <v>74.42202070393374</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -573,7 +573,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>8.977894561109467e-7</v>
+        <v>1.055729522271517</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -581,7 +581,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>18.89623840221119</v>
+        <v>22.220484552705457</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -589,7 +589,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>39.577755237721355</v>
+        <v>39.57775523772136</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -597,7 +597,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.002179714285714286</v>
+        <v>2.179714285714286</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -605,7 +605,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -613,7 +613,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.8444444444444444</v>
+        <v>0.993</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -621,7 +621,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>55.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -637,7 +637,7 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>450.0</v>
+        <v>10000.0</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -645,7 +645,7 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>0.05</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="24" spans="1:2">

</xml_diff>

<commit_message>
modified:   src/ForestInventory.jl 	new file:   src/SIST.jl 	modified:   src/ae.jl 	deleted:    src/as.jl 	modified:   src/qml/main.qml 	modified:   teste.xlsx
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -105,7 +105,7 @@
     <t>Observação</t>
   </si>
   <si>
-    <t>Diante do exposto, conclui-se que os resultados obtidos na amostragem satisfazem as exigências de precisão estabelecidas para o inventário, ou seja, um erro de amostragem máximo de ±10% da média para confiabilidade designada. 
+    <t>Diante do exposto, conclui-se que os resultados obtidos na amostragem satisfazem as exigências de precisão estabelecidas para o inventário, ou seja, um erro de amostragem máximo de ±10.0% da média para confiabilidade designada. 
 O erro estimado foi menor que o limite fixado, assim as unidades amostrais são suficientes para o inventário.</t>
   </si>
 </sst>
@@ -485,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>21.720718880312205</v>
+        <v>19.738614867781166</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>21.720718880312205</v>
+        <v>23.85228004796837</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -501,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>217971.42857142858</v>
+        <v>9.808714285714287e6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -509,7 +509,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>217971.42857142858</v>
+        <v>8.883139620172167e6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -517,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>217971.42857142858</v>
+        <v>1.0734288951256407e7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -525,7 +525,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>4.71386089662237</v>
+        <v>4.7300785974072035</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -533,7 +533,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>1.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -541,7 +541,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.0</v>
+        <v>2.0568325900936015</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -549,7 +549,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>1.0274869937237732</v>
+        <v>1.0310219891319874</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -573,7 +573,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>1.055729522271517</v>
+        <v>1.0630063420736795</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -581,7 +581,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>22.220484552705457</v>
+        <v>22.373643537649695</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -605,7 +605,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -613,7 +613,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.993</v>
+        <v>0.9998444444444444</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -621,7 +621,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -637,7 +637,7 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>10000.0</v>
+        <v>450000.0</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -645,7 +645,7 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>1.0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="24" spans="1:2">

</xml_diff>

<commit_message>
modified:   src/AAS.jl modified:   src/SIST.jl 	modified:   teste.xlsx
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -93,7 +93,7 @@
     <t>População</t>
   </si>
   <si>
-    <t>A população avaliada é considerada infinita</t>
+    <t>A população avaliada é considerada finita</t>
   </si>
   <si>
     <t>Número total de unidades amostrais da população</t>
@@ -477,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>21.79714285714286</v>
+        <v>217.97142857142856</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -485,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>19.738614867781166</v>
+        <v>181.39946248662133</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>23.85228004796837</v>
+        <v>219.20437724555507</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -501,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>9.808714285714287e6</v>
+        <v>9808.714285714286</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -509,7 +509,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>8.883139620172167e6</v>
+        <v>8958.103703638277</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -517,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1.0734288951256407e7</v>
+        <v>106593.24867790294</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -525,7 +525,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>4.7300785974072035</v>
+        <v>4.346980377481731</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -541,7 +541,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>2.0568325900936015</v>
+        <v>18.902457379466863</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -549,7 +549,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>1.0310219891319874</v>
+        <v>9.475175228516605</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -557,7 +557,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>8.626819848816465</v>
+        <v>86.26819848816466</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -565,7 +565,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>74.42202070393374</v>
+        <v>7442.202070393374</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -573,7 +573,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>1.0630063420736795</v>
+        <v>89.77894561109467</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -581,7 +581,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>22.373643537649695</v>
+        <v>18.896238402211203</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -589,7 +589,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>39.57775523772136</v>
+        <v>39.57775523772137</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -597,7 +597,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>2.179714285714286</v>
+        <v>21.79714285714286</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -613,7 +613,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.9998444444444444</v>
+        <v>0.8444444444444444</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -621,7 +621,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>62.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -637,7 +637,7 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>450000.0</v>
+        <v>450.0</v>
       </c>
     </row>
     <row r="23" spans="1:2">

</xml_diff>

<commit_message>
modified:   src/AAS.jl 	new file:   src/DE.jl 	modified:   src/ForestInventory.jl 	deleted:    src/ade.jl 	modified:   src/qml/main.qml 	modified:   teste.xlsx
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -485,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>181.39946248662133</v>
+        <v>199.0689711919617</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>219.20437724555507</v>
+        <v>236.8738859508954</v>
       </c>
     </row>
     <row r="5" spans="1:2">

</xml_diff>

<commit_message>
modified:   src/ForestInventory.jl 	modified:   src/IND.jl 	modified:   src/Save.jl 	modified:   src/ad.jl 	modified:   src/art.jl 	modified:   src/qml/main.qml 	modified:   teste.xlsx
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -13,7 +13,10 @@
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
-    <sheet name="Resultados" sheetId="1" r:id="rId1"/>
+    <sheet name="Dados" sheetId="1" r:id="rId1"/>
+    <sheet name="Primeira_ocasião" r:id="rId5" sheetId="2"/>
+    <sheet name="Segunda_ocasião" r:id="rId6" sheetId="3"/>
+    <sheet name="Crescimento_ou_mudança" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+  <si>
+    <t>Unidades</t>
+  </si>
+  <si>
+    <t>Ocasião_1</t>
+  </si>
+  <si>
+    <t>Ocasião_2</t>
+  </si>
   <si>
     <t>Variáveis</t>
   </si>
@@ -51,12 +63,12 @@
     <t>Limite superior do intervalo de confiança para o total (m³)</t>
   </si>
   <si>
-    <t>Erro padrão relativo (%)</t>
-  </si>
-  <si>
     <t>Área da população (ha)</t>
   </si>
   <si>
+    <t>Erro da amostragem relativo (%)</t>
+  </si>
+  <si>
     <t>Erro da amostragem absoluto (m³/ha)</t>
   </si>
   <si>
@@ -72,41 +84,16 @@
     <t>Variância da média (m³/ha)²</t>
   </si>
   <si>
-    <t>Variância da média relativa (%)</t>
-  </si>
-  <si>
-    <t>Coeficiente de variação (%)</t>
-  </si>
-  <si>
-    <t>Limite de erro da amostragem requerido</t>
-  </si>
-  <si>
-    <t>Estimativa mínima de confiança (m³/ha)</t>
-  </si>
-  <si>
-    <t>Fator de correção</t>
-  </si>
-  <si>
-    <t>Tamanho da amostra</t>
-  </si>
-  <si>
-    <t>População</t>
-  </si>
-  <si>
-    <t>A população avaliada é considerada finita</t>
-  </si>
-  <si>
-    <t>Número total de unidades amostrais da população</t>
-  </si>
-  <si>
-    <t>Nível de significância (α)</t>
-  </si>
-  <si>
-    <t>Observação</t>
-  </si>
-  <si>
-    <t>Diante do exposto, conclui-se que os resultados obtidos na amostragem satisfazem as exigências de precisão estabelecidas para o inventário, ou seja, um erro de amostragem máximo de ±10.0% da média para confiabilidade designada. 
-O erro estimado foi menor que o limite fixado, assim as unidades amostrais são suficientes para o inventário.</t>
+    <t>Número total de unidades</t>
+  </si>
+  <si>
+    <t>Nível de de significância (α)</t>
+  </si>
+  <si>
+    <t>Crescimento médio (m³/ha)</t>
+  </si>
+  <si>
+    <t>Crescimento total estimado (m³)</t>
   </si>
 </sst>
 </file>
@@ -458,202 +445,896 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1.0</v>
+      </c>
+      <c r="B2">
+        <v>146.7</v>
+      </c>
+      <c r="C2">
+        <v>330.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2.0</v>
+      </c>
+      <c r="B3">
+        <v>182.1</v>
+      </c>
+      <c r="C3">
+        <v>222.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3.0</v>
+      </c>
+      <c r="B4">
+        <v>258.6</v>
+      </c>
+      <c r="C4">
+        <v>300.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4.0</v>
+      </c>
+      <c r="B5">
+        <v>198.8</v>
+      </c>
+      <c r="C5">
+        <v>293.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5.0</v>
+      </c>
+      <c r="B6">
+        <v>196.7</v>
+      </c>
+      <c r="C6">
+        <v>270.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6.0</v>
+      </c>
+      <c r="B7">
+        <v>155.6</v>
+      </c>
+      <c r="C7">
+        <v>230.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7.0</v>
+      </c>
+      <c r="B8">
+        <v>201.0</v>
+      </c>
+      <c r="C8">
+        <v>312.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8.0</v>
+      </c>
+      <c r="B9">
+        <v>183.8</v>
+      </c>
+      <c r="C9">
+        <v>341.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9.0</v>
+      </c>
+      <c r="B10">
+        <v>212.4</v>
+      </c>
+      <c r="C10">
+        <v>326.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10.0</v>
+      </c>
+      <c r="B11">
+        <v>202.5</v>
+      </c>
+      <c r="C11">
+        <v>46.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11.0</v>
+      </c>
+      <c r="B12">
+        <v>217.5</v>
+      </c>
+      <c r="C12">
+        <v>312.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12.0</v>
+      </c>
+      <c r="B13">
+        <v>138.9</v>
+      </c>
+      <c r="C13">
+        <v>273.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13.0</v>
+      </c>
+      <c r="B14">
+        <v>242.7</v>
+      </c>
+      <c r="C14">
+        <v>272.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14.0</v>
+      </c>
+      <c r="B15">
+        <v>200.0</v>
+      </c>
+      <c r="C15">
+        <v>225.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15.0</v>
+      </c>
+      <c r="B16">
+        <v>208.3</v>
+      </c>
+      <c r="C16">
+        <v>282.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16.0</v>
+      </c>
+      <c r="B17">
+        <v>193.0</v>
+      </c>
+      <c r="C17">
+        <v>233.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17.0</v>
+      </c>
+      <c r="B18">
+        <v>279.3</v>
+      </c>
+      <c r="C18">
+        <v>213.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>18.0</v>
+      </c>
+      <c r="B19">
+        <v>181.0</v>
+      </c>
+      <c r="C19">
+        <v>224.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>19.0</v>
+      </c>
+      <c r="B20">
+        <v>223.4</v>
+      </c>
+      <c r="C20">
+        <v>229.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>20.0</v>
+      </c>
+      <c r="B21">
+        <v>210.4</v>
+      </c>
+      <c r="C21">
+        <v>188.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>21.0</v>
+      </c>
+      <c r="B22">
+        <v>206.1</v>
+      </c>
+      <c r="C22">
+        <v>176.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>22.0</v>
+      </c>
+      <c r="B23">
+        <v>171.2</v>
+      </c>
+      <c r="C23">
+        <v>221.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>23.0</v>
+      </c>
+      <c r="B24">
+        <v>264.4</v>
+      </c>
+      <c r="C24">
+        <v>247.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>24.0</v>
+      </c>
+      <c r="B25">
+        <v>278.6</v>
+      </c>
+      <c r="C25">
+        <v>249.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>25.0</v>
+      </c>
+      <c r="B26">
+        <v>253.3</v>
+      </c>
+      <c r="C26">
+        <v>230.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>26.0</v>
+      </c>
+      <c r="B27">
+        <v>41.0</v>
+      </c>
+      <c r="C27">
+        <v>136.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>27.0</v>
+      </c>
+      <c r="B28">
+        <v>242.9</v>
+      </c>
+      <c r="C28">
+        <v>285.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>28.0</v>
+      </c>
+      <c r="B29">
+        <v>241.6</v>
+      </c>
+      <c r="C29">
+        <v>265.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>29.0</v>
+      </c>
+      <c r="B30">
+        <v>251.2</v>
+      </c>
+      <c r="C30">
+        <v>248.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>30.0</v>
+      </c>
+      <c r="B31">
+        <v>144.5</v>
+      </c>
+      <c r="C31">
+        <v>250.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>31.0</v>
+      </c>
+      <c r="B32">
+        <v>225.9</v>
+      </c>
+      <c r="C32">
+        <v>238.0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>32.0</v>
+      </c>
+      <c r="B33">
+        <v>178.5</v>
+      </c>
+      <c r="C33">
+        <v>265.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>33.0</v>
+      </c>
+      <c r="B34">
+        <v>182.0</v>
+      </c>
+      <c r="C34">
+        <v>210.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>34.0</v>
+      </c>
+      <c r="B35">
+        <v>176.2</v>
+      </c>
+      <c r="C35">
+        <v>280.0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>35.0</v>
+      </c>
+      <c r="B36">
+        <v>199.5</v>
+      </c>
+      <c r="C36">
+        <v>198.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>36.0</v>
+      </c>
+      <c r="B37">
+        <v>156.8</v>
+      </c>
+      <c r="C37">
+        <v>290.3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>37.0</v>
+      </c>
+      <c r="B38">
+        <v>136.2</v>
+      </c>
+      <c r="C38">
+        <v>248.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>38.0</v>
+      </c>
+      <c r="B39">
+        <v>225.4</v>
+      </c>
+      <c r="C39">
+        <v>235.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>39.0</v>
+      </c>
+      <c r="B40">
+        <v>184.3</v>
+      </c>
+      <c r="C40">
+        <v>265.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>40.0</v>
+      </c>
+      <c r="B41">
+        <v>245.8</v>
+      </c>
+      <c r="C41">
+        <v>236.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>41.0</v>
+      </c>
+      <c r="B42">
+        <v>164.9</v>
+      </c>
+      <c r="C42">
+        <v>280.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>42.0</v>
+      </c>
+      <c r="B43">
+        <v>198.8</v>
+      </c>
+      <c r="C43">
+        <v>285.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>43.0</v>
+      </c>
+      <c r="B44">
+        <v>168.6</v>
+      </c>
+      <c r="C44">
+        <v>198.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>44.0</v>
+      </c>
+      <c r="B45">
+        <v>228.7</v>
+      </c>
+      <c r="C45">
+        <v>248.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>217.97142857142856</v>
+        <v>199.97954545454547</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>199.0689711919617</v>
+        <v>186.8278944029383</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>236.8738859508954</v>
+        <v>213.13119650615263</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>9808.714285714286</v>
+        <v>299969.31818181823</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>8958.103703638277</v>
+        <v>280241.8416044075</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>106593.24867790294</v>
+        <v>319696.79475922894</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>4.346980377481731</v>
+        <v>1500.0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>45.0</v>
+        <v>6.5764981222024375</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>18.902457379466863</v>
+        <v>13.151651051607152</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>9.475175228516605</v>
+        <v>6.52139729436293</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>86.26819848816466</v>
+        <v>43.906815476050355</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B13">
-        <v>7442.202070393374</v>
+        <v>1927.808445247935</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>89.77894561109467</v>
+        <v>42.52862267092414</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>18.896238402211203</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>248.1886363636364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>232.6224520290209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>263.7548206982519</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>372282.9545454546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>348933.67804353137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>395632.2310473778</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>6.271916620633878</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>15.566184334615485</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>7.718671367190127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>51.96774006276784</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
+      <c r="B13">
+        <v>2700.6460072314053</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>59.577887674680696</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>44.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
       <c r="B16">
-        <v>39.57775523772137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>48.20909090909092</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>28.118087862453574</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>68.30009395572826</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>72313.63636363638</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>42177.13179368037</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>102450.1409335924</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>41.67471874656057</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>20.091003046637343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>10.104776610376147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
-        <v>21.79714285714286</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>0.8444444444444444</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>55.0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22">
-        <v>450.0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
+      <c r="B12">
+        <v>102.10651034560485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>